<commit_message>
added products to seed & removed id from model
</commit_message>
<xml_diff>
--- a/server/db/data/mockData.xlsx
+++ b/server/db/data/mockData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerposner/Desktop/fullstack-academy/grace-shopper/server/db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E5219-D5D0-BA46-861A-9A389DB64A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC08507-B5DE-A14D-A4AE-844A594B715A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" activeTab="2" xr2:uid="{38C6CE76-0E72-CE4F-8F7D-45C061201DCA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -45,31 +45,31 @@
     <t>imageUrl</t>
   </si>
   <si>
-    <t>Product 1</t>
-  </si>
-  <si>
-    <t>Product 2</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>cate</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>productId</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
     <t>available</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Grey T-Shirt</t>
+  </si>
+  <si>
+    <t>Black T-Shirt</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
 </sst>
 </file>
@@ -430,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A372BC8-F725-AF45-92B0-F12A4933BA9C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,27 +448,42 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -478,20 +493,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2916BAB5-85C8-FA4A-8EF2-0092F580CE2A}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F3B66F-CF6D-7841-BEC6-DE5D7E631605}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -499,54 +544,47 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F3B66F-CF6D-7841-BEC6-DE5D7E631605}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed heading to camping-grace
</commit_message>
<xml_diff>
--- a/server/db/data/mockData.xlsx
+++ b/server/db/data/mockData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerposner/Desktop/fullstack-academy/grace-shopper/server/db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F13CE3D-F3AF-AC42-BD8E-3E8C80187298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343F59EC-6335-BF4B-A549-73EF794E99C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" xr2:uid="{38C6CE76-0E72-CE4F-8F7D-45C061201DCA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>product</t>
+  </si>
+  <si>
+    <t>Slacks</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A372BC8-F725-AF45-92B0-F12A4933BA9C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,6 +488,17 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added imageUrl to seed
</commit_message>
<xml_diff>
--- a/server/db/data/mockData.xlsx
+++ b/server/db/data/mockData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerposner/Desktop/fullstack-academy/grace-shopper/server/db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0769C6E7-7CC6-F748-BF31-ABDA17A8422D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9DBE67-176D-3E45-A73D-50CE0E1CCFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" xr2:uid="{38C6CE76-0E72-CE4F-8F7D-45C061201DCA}"/>
   </bookViews>
@@ -756,7 +756,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated imageUrl with extension
</commit_message>
<xml_diff>
--- a/server/db/data/mockData.xlsx
+++ b/server/db/data/mockData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerposner/Desktop/fullstack-academy/grace-shopper/server/db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9DBE67-176D-3E45-A73D-50CE0E1CCFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB90D0-C348-0A4F-811D-9DE8FDE6C029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15900" xr2:uid="{38C6CE76-0E72-CE4F-8F7D-45C061201DCA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="10000" windowHeight="15900" xr2:uid="{38C6CE76-0E72-CE4F-8F7D-45C061201DCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -59,312 +59,171 @@
     <t>Snap Long Sleeve Shirt</t>
   </si>
   <si>
-    <t>shirts/clsh-1</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, est et oporteat interpretaris. An malis volumus convenire est</t>
   </si>
   <si>
     <t>Mossy Long Sleeve Shirt</t>
   </si>
   <si>
-    <t>shirts/clsh-2</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, et impetus civibus mea, luptatum sententiae omittantur pro id.</t>
   </si>
   <si>
     <t>Rancher Long Sleeve Shirt</t>
   </si>
   <si>
-    <t>shirts/clsh-3</t>
-  </si>
-  <si>
     <t>Fleece Driver Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-1</t>
-  </si>
-  <si>
     <t>Eum quas legimus invidunt ad, ne eam putent feugiat facilis. Ne vis impedit antiopam torquatos, vim case nostrud no.</t>
   </si>
   <si>
     <t>Brick Vest</t>
   </si>
   <si>
-    <t>outerwear/clou-3</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, nemore iisque lucilius sed eu, sed mentitum nominati percipitur ne, idque molestie vix in. </t>
   </si>
   <si>
     <t>Mason Parka</t>
   </si>
   <si>
-    <t>outerwear/clou-2</t>
-  </si>
-  <si>
     <t>Wooly Hoody</t>
   </si>
   <si>
-    <t>outerwear/clou-4</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, quo reque accusam at, pri diam denique facilisis no.</t>
   </si>
   <si>
     <t>Lodger Reversible Vest</t>
   </si>
   <si>
-    <t>outerwear/clou-5</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, pri incorrupte concludaturque te.</t>
   </si>
   <si>
     <t>Rain Zapper Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-6</t>
-  </si>
-  <si>
     <t>Wooly Coat</t>
   </si>
   <si>
-    <t>outerwear/clou-7</t>
-  </si>
-  <si>
     <t>Brick Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-8</t>
-  </si>
-  <si>
     <t>Brick and Mortar Reversible Parka</t>
   </si>
   <si>
-    <t>outerwear/clou-9</t>
-  </si>
-  <si>
     <t>Wooly Parka</t>
   </si>
   <si>
-    <t>outerwear/clou-10</t>
-  </si>
-  <si>
     <t>Red Noise Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-11</t>
-  </si>
-  <si>
     <t>Space Blender Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-12</t>
-  </si>
-  <si>
     <t>Brick Windy Hoody</t>
   </si>
   <si>
-    <t>outerwear/clou-13</t>
-  </si>
-  <si>
     <t>Cabin Canvas Jacket</t>
   </si>
   <si>
-    <t>outerwear/clou-14</t>
-  </si>
-  <si>
     <t>Barker Denim Overalls</t>
   </si>
   <si>
-    <t>pants/clpa-1</t>
-  </si>
-  <si>
     <t>Slip Wader Overalls</t>
   </si>
   <si>
-    <t>pants/clpa-2</t>
-  </si>
-  <si>
     <t>Indigo Pants</t>
   </si>
   <si>
-    <t>pants/clpa-3</t>
-  </si>
-  <si>
     <t>Straight Jeans</t>
   </si>
   <si>
-    <t>pants/clpa-4</t>
-  </si>
-  <si>
     <t>Blue Denim Overalls</t>
   </si>
   <si>
-    <t>pants/clpa-5</t>
-  </si>
-  <si>
     <t>Denim Carpenter Jeans</t>
   </si>
   <si>
-    <t>pants/clpa-6</t>
-  </si>
-  <si>
     <t>One Piece Coveralls</t>
   </si>
   <si>
-    <t>pants/clpa-7</t>
-  </si>
-  <si>
     <t>Slate Convertible Pants</t>
   </si>
   <si>
-    <t>pants/clpa-8</t>
-  </si>
-  <si>
     <t>Blue Joggers</t>
   </si>
   <si>
-    <t>pants/clpa-9</t>
-  </si>
-  <si>
     <t>Dusty Crops</t>
   </si>
   <si>
-    <t>pants/clpa-10</t>
-  </si>
-  <si>
     <t>Lagoon Longsleeve</t>
   </si>
   <si>
-    <t>shirts/clsh-4</t>
-  </si>
-  <si>
     <t>Kahki Range Longsleeve</t>
   </si>
   <si>
-    <t>shirts/clsh-5</t>
-  </si>
-  <si>
     <t>Treeline Zip-Neck Longsleeve</t>
   </si>
   <si>
-    <t>shirts/clsh-6</t>
-  </si>
-  <si>
     <t>Green Herring Pullover Longsleeve</t>
   </si>
   <si>
-    <t>shirts/clsh-7</t>
-  </si>
-  <si>
     <t>Slipstream Waders</t>
   </si>
   <si>
-    <t>accessories/clac-6</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, his et case percipit maiestatis, tempor vivendum sea an. </t>
   </si>
   <si>
     <t>River Wading Boots</t>
   </si>
   <si>
-    <t>accessories/clac-3</t>
-  </si>
-  <si>
     <t>River Wading Socks</t>
   </si>
   <si>
-    <t>accessories/clac-5</t>
-  </si>
-  <si>
     <t>River Belt</t>
   </si>
   <si>
-    <t>accessories/clac-2</t>
-  </si>
-  <si>
     <t>River Boots</t>
   </si>
   <si>
-    <t>accessories/clac-4</t>
-  </si>
-  <si>
     <t>Downstream Waders</t>
   </si>
   <si>
-    <t>accessories/clac-1</t>
-  </si>
-  <si>
     <t>Shortstack Beanie</t>
   </si>
   <si>
-    <t>accessories/clac-7</t>
-  </si>
-  <si>
     <t>Goldeneye Trucker Hat</t>
   </si>
   <si>
-    <t>accessories/clac-8</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, iuvaret forensibus no eos.</t>
   </si>
   <si>
     <t>Dark Bucket Hat</t>
   </si>
   <si>
-    <t>accessories/clac-9</t>
-  </si>
-  <si>
     <t>Light Grey Tent</t>
   </si>
   <si>
-    <t>gear/gear-1</t>
-  </si>
-  <si>
     <t>gear</t>
   </si>
   <si>
     <t>Medium Green Tent</t>
   </si>
   <si>
-    <t>gear/gear-2</t>
-  </si>
-  <si>
     <t>Large Green Tent</t>
   </si>
   <si>
-    <t>gear/gear-3</t>
-  </si>
-  <si>
     <t>Canopy Hammock</t>
   </si>
   <si>
-    <t>gear/gear-4</t>
-  </si>
-  <si>
     <t>Cozy Tent</t>
   </si>
   <si>
-    <t>gear/gear-5</t>
-  </si>
-  <si>
     <t>Breezy Tent</t>
   </si>
   <si>
-    <t>gear/gear-6</t>
-  </si>
-  <si>
     <t>Hiking Backpack</t>
   </si>
   <si>
-    <t>gear/gear-7</t>
-  </si>
-  <si>
     <t>shirts</t>
   </si>
   <si>
@@ -378,6 +237,147 @@
   </si>
   <si>
     <t>productId</t>
+  </si>
+  <si>
+    <t>accessories/clac-1.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-7.webp</t>
+  </si>
+  <si>
+    <t>accessories/clac-8.webp</t>
+  </si>
+  <si>
+    <t>accessories/clac-9.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-6.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-3.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-5.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-2.jpg</t>
+  </si>
+  <si>
+    <t>accessories/clac-4.jpg</t>
+  </si>
+  <si>
+    <t>gear/gear-1.png</t>
+  </si>
+  <si>
+    <t>gear/gear-2.png</t>
+  </si>
+  <si>
+    <t>gear/gear-3.png</t>
+  </si>
+  <si>
+    <t>gear/gear-4.jpg</t>
+  </si>
+  <si>
+    <t>gear/gear-5.jpg</t>
+  </si>
+  <si>
+    <t>gear/gear-6.jpg</t>
+  </si>
+  <si>
+    <t>gear/gear-7.jpg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-1.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-3.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-2.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-4.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-5.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-6.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-7.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-8.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-9.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-10.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-11.jpg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-12.jpeg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-13.jpg</t>
+  </si>
+  <si>
+    <t>outerwear/clou-14.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-1.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-2.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-3.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-4.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-5.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-6.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-7.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-8.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-9.jpg</t>
+  </si>
+  <si>
+    <t>pants/clpa-10.jpg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-1.jpeg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-2.jpeg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-3.jpeg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-4.jpg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-5.jpg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-6.jpg</t>
+  </si>
+  <si>
+    <t>shirts/clsh-7.jpg</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,795 +791,795 @@
         <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>189</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>149</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>399</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
         <v>159</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3">
         <v>189</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3">
         <v>289</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3">
         <v>259</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3">
         <v>229</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3">
         <v>399</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3">
         <v>199</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3">
         <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3">
         <v>239</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3">
         <v>149</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3">
         <v>111</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3">
         <v>229</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3">
         <v>229</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3">
         <v>199</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3">
         <v>119</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3">
         <v>229</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3">
         <v>219</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3">
         <v>249</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3">
         <v>259</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3">
         <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3">
         <v>115</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B29" s="3">
         <v>79</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="B30" s="3">
         <v>119</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3">
         <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3">
         <v>79</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B33" s="3">
         <v>399</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B34" s="3">
         <v>249</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B35" s="3">
         <v>229</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B36" s="3">
         <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="B37" s="3">
         <v>249</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="B38" s="3">
         <v>399</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3">
         <v>24</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B40" s="3">
         <v>24</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B41" s="3">
         <v>11</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B42" s="3">
         <v>289</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B43" s="3">
         <v>339</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B44" s="3">
         <v>425</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="B45" s="3">
         <v>89</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="B46" s="3">
         <v>99</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B47" s="3">
         <v>99</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="B48" s="3">
         <v>115</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
@@ -1605,7 +1605,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>

</xml_diff>